<commit_message>
New ids for series and indicators
</commit_message>
<xml_diff>
--- a/master_data/catalog_series_old_and_new.xlsx
+++ b/master_data/catalog_series_old_and_new.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gonzalezmorales\projects\ARCGIS HUBS\gender_data_portal\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gonzalezmorales\projects\ARCGIS HUBS\gender_data_portal\master_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E17B9237-3AA2-4A32-81FF-A039D84F92F0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC35898D-23DA-4530-A8BE-81ECDF5C6FF9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="879" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="879" uniqueCount="431">
   <si>
     <t>INDICATOR_ID</t>
   </si>
@@ -1283,6 +1283,39 @@
   </si>
   <si>
     <t>PDM</t>
+  </si>
+  <si>
+    <t>I.1q</t>
+  </si>
+  <si>
+    <t>I.2q</t>
+  </si>
+  <si>
+    <t>I.3q</t>
+  </si>
+  <si>
+    <t>I.4q</t>
+  </si>
+  <si>
+    <t>IV.1q</t>
+  </si>
+  <si>
+    <t>IV.2q</t>
+  </si>
+  <si>
+    <t>IV.3q</t>
+  </si>
+  <si>
+    <t>V.1q</t>
+  </si>
+  <si>
+    <t>V.2q</t>
+  </si>
+  <si>
+    <t>V.3q</t>
+  </si>
+  <si>
+    <t>V.4q</t>
   </si>
 </sst>
 </file>
@@ -2185,8 +2218,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M125" sqref="M125"/>
+    <sheetView tabSelected="1" topLeftCell="A111" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F126" sqref="F126:F127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5884,7 +5917,7 @@
         <v>348</v>
       </c>
       <c r="F89" s="4" t="s">
-        <v>81</v>
+        <v>420</v>
       </c>
       <c r="G89" s="4" t="s">
         <v>349</v>
@@ -5926,7 +5959,7 @@
         <v>348</v>
       </c>
       <c r="F90" s="4" t="s">
-        <v>81</v>
+        <v>420</v>
       </c>
       <c r="G90" s="4" t="s">
         <v>350</v>
@@ -5968,7 +6001,7 @@
         <v>351</v>
       </c>
       <c r="F91" s="4" t="s">
-        <v>91</v>
+        <v>421</v>
       </c>
       <c r="G91" s="4" t="s">
         <v>352</v>
@@ -6010,7 +6043,7 @@
         <v>351</v>
       </c>
       <c r="F92" s="4" t="s">
-        <v>91</v>
+        <v>421</v>
       </c>
       <c r="G92" s="4" t="s">
         <v>353</v>
@@ -6052,7 +6085,7 @@
         <v>351</v>
       </c>
       <c r="F93" s="4" t="s">
-        <v>91</v>
+        <v>421</v>
       </c>
       <c r="G93" s="4" t="s">
         <v>354</v>
@@ -6094,7 +6127,7 @@
         <v>351</v>
       </c>
       <c r="F94" s="4" t="s">
-        <v>91</v>
+        <v>421</v>
       </c>
       <c r="G94" s="4" t="s">
         <v>355</v>
@@ -6136,7 +6169,7 @@
         <v>79580982</v>
       </c>
       <c r="F95" s="4" t="s">
-        <v>94</v>
+        <v>422</v>
       </c>
       <c r="G95" s="4">
         <v>79580982</v>
@@ -6178,7 +6211,7 @@
         <v>356</v>
       </c>
       <c r="F96" s="4" t="s">
-        <v>100</v>
+        <v>423</v>
       </c>
       <c r="G96" s="4" t="s">
         <v>356</v>
@@ -6220,7 +6253,7 @@
         <v>357</v>
       </c>
       <c r="F97" s="4" t="s">
-        <v>285</v>
+        <v>424</v>
       </c>
       <c r="G97" s="4" t="s">
         <v>357</v>
@@ -6262,7 +6295,7 @@
         <v>358</v>
       </c>
       <c r="F98" s="4" t="s">
-        <v>290</v>
+        <v>425</v>
       </c>
       <c r="G98" s="4" t="s">
         <v>358</v>
@@ -6304,7 +6337,7 @@
         <v>359</v>
       </c>
       <c r="F99" s="4" t="s">
-        <v>298</v>
+        <v>426</v>
       </c>
       <c r="G99" s="4" t="s">
         <v>359</v>
@@ -6342,7 +6375,7 @@
         <v>360</v>
       </c>
       <c r="F100" s="4" t="s">
-        <v>325</v>
+        <v>427</v>
       </c>
       <c r="G100" s="4" t="s">
         <v>360</v>
@@ -6382,7 +6415,7 @@
         <v>360</v>
       </c>
       <c r="F101" s="4" t="s">
-        <v>325</v>
+        <v>427</v>
       </c>
       <c r="G101" s="4">
         <v>17230409</v>
@@ -6422,7 +6455,7 @@
         <v>360</v>
       </c>
       <c r="F102" s="4" t="s">
-        <v>325</v>
+        <v>427</v>
       </c>
       <c r="G102" s="4" t="s">
         <v>363</v>
@@ -6462,7 +6495,7 @@
         <v>360</v>
       </c>
       <c r="F103" s="4" t="s">
-        <v>325</v>
+        <v>427</v>
       </c>
       <c r="G103" s="4" t="s">
         <v>365</v>
@@ -6502,7 +6535,7 @@
         <v>360</v>
       </c>
       <c r="F104" s="4" t="s">
-        <v>325</v>
+        <v>427</v>
       </c>
       <c r="G104" s="4" t="s">
         <v>367</v>
@@ -6542,7 +6575,7 @@
         <v>360</v>
       </c>
       <c r="F105" s="4" t="s">
-        <v>325</v>
+        <v>427</v>
       </c>
       <c r="G105" s="4" t="s">
         <v>369</v>
@@ -6582,7 +6615,7 @@
         <v>360</v>
       </c>
       <c r="F106" s="4" t="s">
-        <v>325</v>
+        <v>427</v>
       </c>
       <c r="G106" s="4" t="s">
         <v>371</v>
@@ -6622,7 +6655,7 @@
         <v>360</v>
       </c>
       <c r="F107" s="4" t="s">
-        <v>325</v>
+        <v>427</v>
       </c>
       <c r="G107" s="4" t="s">
         <v>373</v>
@@ -6662,7 +6695,7 @@
         <v>360</v>
       </c>
       <c r="F108" s="4" t="s">
-        <v>325</v>
+        <v>427</v>
       </c>
       <c r="G108" s="4" t="s">
         <v>375</v>
@@ -6702,7 +6735,7 @@
         <v>360</v>
       </c>
       <c r="F109" s="4" t="s">
-        <v>325</v>
+        <v>427</v>
       </c>
       <c r="G109" s="4" t="s">
         <v>377</v>
@@ -6736,7 +6769,7 @@
         <v>379</v>
       </c>
       <c r="F110" s="4" t="s">
-        <v>325</v>
+        <v>427</v>
       </c>
       <c r="G110" s="4" t="s">
         <v>380</v>
@@ -6772,7 +6805,7 @@
         <v>379</v>
       </c>
       <c r="F111" s="4" t="s">
-        <v>325</v>
+        <v>427</v>
       </c>
       <c r="G111" s="4" t="s">
         <v>383</v>
@@ -6808,7 +6841,7 @@
         <v>379</v>
       </c>
       <c r="F112" s="4" t="s">
-        <v>325</v>
+        <v>427</v>
       </c>
       <c r="G112" s="4" t="s">
         <v>386</v>
@@ -6844,7 +6877,7 @@
         <v>379</v>
       </c>
       <c r="F113" s="4" t="s">
-        <v>325</v>
+        <v>427</v>
       </c>
       <c r="G113" s="4" t="s">
         <v>389</v>
@@ -6884,7 +6917,7 @@
         <v>392</v>
       </c>
       <c r="F114" s="4" t="s">
-        <v>329</v>
+        <v>428</v>
       </c>
       <c r="G114" s="4" t="s">
         <v>393</v>
@@ -6926,7 +6959,7 @@
         <v>392</v>
       </c>
       <c r="F115" s="4" t="s">
-        <v>329</v>
+        <v>428</v>
       </c>
       <c r="G115" s="4" t="s">
         <v>392</v>
@@ -6966,7 +6999,7 @@
         <v>392</v>
       </c>
       <c r="F116" s="4" t="s">
-        <v>329</v>
+        <v>428</v>
       </c>
       <c r="G116" s="4" t="s">
         <v>396</v>
@@ -7006,7 +7039,7 @@
         <v>392</v>
       </c>
       <c r="F117" s="4" t="s">
-        <v>329</v>
+        <v>428</v>
       </c>
       <c r="G117" s="4" t="s">
         <v>397</v>
@@ -7044,7 +7077,7 @@
         <v>398</v>
       </c>
       <c r="F118" s="4" t="s">
-        <v>333</v>
+        <v>429</v>
       </c>
       <c r="G118" s="4" t="s">
         <v>398</v>
@@ -7088,7 +7121,7 @@
         <v>398</v>
       </c>
       <c r="F119" s="4" t="s">
-        <v>333</v>
+        <v>429</v>
       </c>
       <c r="G119" s="4" t="s">
         <v>400</v>
@@ -7130,7 +7163,7 @@
         <v>398</v>
       </c>
       <c r="F120" s="4" t="s">
-        <v>333</v>
+        <v>429</v>
       </c>
       <c r="G120" s="4" t="s">
         <v>401</v>
@@ -7170,7 +7203,7 @@
         <v>402</v>
       </c>
       <c r="F121" s="4" t="s">
-        <v>336</v>
+        <v>430</v>
       </c>
       <c r="G121" s="4" t="s">
         <v>402</v>
@@ -7210,7 +7243,7 @@
         <v>402</v>
       </c>
       <c r="F122" s="4" t="s">
-        <v>336</v>
+        <v>430</v>
       </c>
       <c r="G122" s="4" t="s">
         <v>404</v>
@@ -7252,7 +7285,7 @@
         <v>402</v>
       </c>
       <c r="F123" s="4" t="s">
-        <v>336</v>
+        <v>430</v>
       </c>
       <c r="G123" s="4" t="s">
         <v>406</v>

</xml_diff>

<commit_message>
fix codes and duplicates
</commit_message>
<xml_diff>
--- a/master_data/catalog_series_old_and_new.xlsx
+++ b/master_data/catalog_series_old_and_new.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gonzalezmorales\projects\ARCGIS HUBS\gender_data_portal\master_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C43947C-7717-4DF0-8E96-5FEB93AC5FD2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59282557-665F-44E5-A739-3026D3CB1555}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25080" yWindow="8805" windowWidth="29040" windowHeight="15840" xr2:uid="{DE7C0272-EBF5-4B5F-81CF-57D56F39C38E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{DE7C0272-EBF5-4B5F-81CF-57D56F39C38E}"/>
   </bookViews>
   <sheets>
     <sheet name="CL_SERIES" sheetId="1" r:id="rId1"/>
@@ -729,9 +729,6 @@
     <t>SH_FPL_INFM</t>
   </si>
   <si>
-    <t xml:space="preserve">	bef52966</t>
-  </si>
-  <si>
     <t>Proportion of women who make their own informed decisions regarding contraceptive use (% of women aged 15-49 years)</t>
   </si>
   <si>
@@ -747,9 +744,6 @@
     <t>SH_FPL_INFMRH</t>
   </si>
   <si>
-    <t xml:space="preserve">	91c32905</t>
-  </si>
-  <si>
     <t>Proportion of women who make their own informed decisions regarding sexual relations (% of women aged 15-49 years)</t>
   </si>
   <si>
@@ -1227,15 +1221,9 @@
     <t>S6bcc3b15</t>
   </si>
   <si>
-    <t>S	bef52966</t>
-  </si>
-  <si>
     <t>Sf8af2bef</t>
   </si>
   <si>
-    <t>S	91c32905</t>
-  </si>
-  <si>
     <t>S9a5e3c3a</t>
   </si>
   <si>
@@ -1606,6 +1594,18 @@
   </si>
   <si>
     <t>If1e8239d</t>
+  </si>
+  <si>
+    <t>bef52966</t>
+  </si>
+  <si>
+    <t>Sbef52966</t>
+  </si>
+  <si>
+    <t>S91c32905</t>
+  </si>
+  <si>
+    <t>91c32905</t>
   </si>
 </sst>
 </file>
@@ -2242,8 +2242,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17A2D352-C4C8-4DE2-97CA-D08B75E57DA1}">
   <dimension ref="A1:P123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.42578125" defaultRowHeight="12.75"/>
@@ -2264,22 +2264,22 @@
   <sheetData>
     <row r="1" spans="1:16" ht="25.5">
       <c r="A1" s="29" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="B1" s="30" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="29" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>1</v>
@@ -2300,16 +2300,16 @@
         <v>6</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="63.75">
@@ -2324,13 +2324,13 @@
         <v>100</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>8</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>9</v>
@@ -2363,13 +2363,13 @@
         <v>200</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>8</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>13</v>
@@ -2402,13 +2402,13 @@
         <v>300</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>8</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>15</v>
@@ -2441,13 +2441,13 @@
         <v>400</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>17</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>18</v>
@@ -2478,13 +2478,13 @@
         <v>500</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>19</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>20</v>
@@ -2518,13 +2518,13 @@
         <v>600</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>19</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>23</v>
@@ -2558,13 +2558,13 @@
         <v>700</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>24</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="H8" s="4" t="s">
         <v>25</v>
@@ -2598,13 +2598,13 @@
         <v>800</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>27</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>28</v>
@@ -2638,13 +2638,13 @@
         <v>900</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>29</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="H10" s="4" t="s">
         <v>30</v>
@@ -2677,13 +2677,13 @@
         <v>1000</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="F11" s="15" t="s">
         <v>32</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H11" s="15" t="s">
         <v>34</v>
@@ -2716,11 +2716,11 @@
         <v>1100</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="11" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>37</v>
@@ -2751,13 +2751,13 @@
         <v>1200</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>38</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>39</v>
@@ -2788,13 +2788,13 @@
         <v>1300</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>38</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="H14" s="4" t="s">
         <v>42</v>
@@ -2828,13 +2828,13 @@
         <v>1400</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>38</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="H15" s="4" t="s">
         <v>43</v>
@@ -2868,13 +2868,13 @@
         <v>1500</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>44</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="H16" s="4" t="s">
         <v>45</v>
@@ -2907,11 +2907,11 @@
         <v>1600</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="11" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="H17" s="4" t="s">
         <v>47</v>
@@ -2944,13 +2944,13 @@
         <v>1700</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>50</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="H18" s="4" t="s">
         <v>51</v>
@@ -2983,13 +2983,13 @@
         <v>1800</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>50</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="H19" s="4" t="s">
         <v>52</v>
@@ -3025,13 +3025,13 @@
         <v>1900</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>54</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="H20" s="4" t="s">
         <v>55</v>
@@ -3064,13 +3064,13 @@
         <v>2000</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>58</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="H21" s="4" t="s">
         <v>59</v>
@@ -3104,13 +3104,13 @@
         <v>2100</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>60</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="H22" s="4" t="s">
         <v>61</v>
@@ -3142,13 +3142,13 @@
         <v>2200</v>
       </c>
       <c r="E23" s="18" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="F23" s="19" t="s">
         <v>60</v>
       </c>
       <c r="G23" s="20" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="H23" s="19" t="s">
         <v>64</v>
@@ -3177,13 +3177,13 @@
         <v>2300</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>65</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="H24" s="4" t="s">
         <v>66</v>
@@ -3216,13 +3216,13 @@
         <v>2400</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="F25" s="15" t="s">
         <v>69</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="H25" s="15" t="s">
         <v>71</v>
@@ -3253,13 +3253,13 @@
         <v>2500</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="F26" s="15" t="s">
         <v>69</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="H26" s="15" t="s">
         <v>74</v>
@@ -3293,11 +3293,11 @@
         <v>2600</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="F27" s="4"/>
       <c r="G27" s="11" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="H27" s="4" t="s">
         <v>75</v>
@@ -3318,7 +3318,7 @@
     </row>
     <row r="28" spans="1:16" ht="51">
       <c r="A28" s="14" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="12" t="s">
@@ -3328,13 +3328,13 @@
         <v>2700</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="F28" s="15" t="s">
         <v>77</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="H28" s="15" t="s">
         <v>78</v>
@@ -3368,11 +3368,11 @@
         <v>2800</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="F29" s="4"/>
       <c r="G29" s="11" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="H29" s="4" t="s">
         <v>80</v>
@@ -3400,13 +3400,13 @@
         <v>2900</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="F30" s="4" t="s">
         <v>81</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="H30" s="4" t="s">
         <v>82</v>
@@ -3436,13 +3436,13 @@
         <v>3000</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>83</v>
       </c>
       <c r="G31" s="11" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="H31" s="4" t="s">
         <v>84</v>
@@ -3475,11 +3475,11 @@
         <v>3100</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="F32" s="4"/>
       <c r="G32" s="11" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="H32" s="4" t="s">
         <v>86</v>
@@ -3492,7 +3492,7 @@
         <v>5</v>
       </c>
       <c r="N32" s="7" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="O32" s="22"/>
       <c r="P32" s="23"/>
@@ -3509,13 +3509,13 @@
         <v>3200</v>
       </c>
       <c r="E33" s="14" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="F33" s="15" t="s">
         <v>115</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="H33" s="15" t="s">
         <v>117</v>
@@ -3548,11 +3548,11 @@
         <v>3300</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="F34" s="4"/>
       <c r="G34" s="11" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="H34" s="4" t="s">
         <v>96</v>
@@ -3567,7 +3567,7 @@
         <v>5</v>
       </c>
       <c r="N34" s="7" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="O34" s="7"/>
       <c r="P34" s="6"/>
@@ -3584,13 +3584,13 @@
         <v>3400</v>
       </c>
       <c r="E35" s="18" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="F35" s="19" t="s">
         <v>93</v>
       </c>
       <c r="G35" s="20" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="H35" s="19" t="s">
         <v>94</v>
@@ -3622,13 +3622,13 @@
         <v>3500</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="F36" s="4" t="s">
         <v>97</v>
       </c>
       <c r="G36" s="11" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="H36" s="4" t="s">
         <v>98</v>
@@ -3662,13 +3662,13 @@
         <v>3600</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="F37" s="4" t="s">
         <v>100</v>
       </c>
       <c r="G37" s="11" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="H37" s="4" t="s">
         <v>101</v>
@@ -3702,11 +3702,11 @@
         <v>3700</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="F38" s="4"/>
       <c r="G38" s="11" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="H38" s="4" t="s">
         <v>103</v>
@@ -3722,7 +3722,7 @@
         <v>5</v>
       </c>
       <c r="N38" s="7" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="39" spans="1:16" ht="51">
@@ -3737,11 +3737,11 @@
         <v>3800</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="F39" s="4"/>
       <c r="G39" s="11" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="H39" s="4" t="s">
         <v>105</v>
@@ -3757,7 +3757,7 @@
         <v>5</v>
       </c>
       <c r="N39" s="7" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="40" spans="1:16" ht="63.75">
@@ -3772,11 +3772,11 @@
         <v>3900</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="F40" s="4"/>
       <c r="G40" s="11" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="H40" s="4" t="s">
         <v>107</v>
@@ -3792,7 +3792,7 @@
         <v>5</v>
       </c>
       <c r="N40" s="7" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="41" spans="1:16" ht="51">
@@ -3807,11 +3807,11 @@
         <v>4000</v>
       </c>
       <c r="E41" s="10" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="F41" s="4"/>
       <c r="G41" s="11" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="H41" s="4" t="s">
         <v>109</v>
@@ -3824,7 +3824,7 @@
         <v>5</v>
       </c>
       <c r="N41" s="7" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="42" spans="1:16" ht="63.75">
@@ -3839,11 +3839,11 @@
         <v>4100</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="F42" s="4"/>
       <c r="G42" s="11" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="H42" s="4" t="s">
         <v>110</v>
@@ -3856,7 +3856,7 @@
         <v>5</v>
       </c>
       <c r="N42" s="7" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="43" spans="1:16" ht="51">
@@ -3871,11 +3871,11 @@
         <v>4200</v>
       </c>
       <c r="E43" s="10" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="F43" s="4"/>
       <c r="G43" s="11" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="H43" s="4" t="s">
         <v>119</v>
@@ -3888,7 +3888,7 @@
         <v>5</v>
       </c>
       <c r="N43" s="7" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="44" spans="1:16" ht="51">
@@ -3903,13 +3903,13 @@
         <v>4300</v>
       </c>
       <c r="E44" s="14" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="F44" s="15" t="s">
         <v>121</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="H44" s="15" t="s">
         <v>123</v>
@@ -3941,11 +3941,11 @@
         <v>4400</v>
       </c>
       <c r="E45" s="10" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="F45" s="4"/>
       <c r="G45" s="11" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="H45" s="4" t="s">
         <v>125</v>
@@ -3958,7 +3958,7 @@
         <v>5</v>
       </c>
       <c r="N45" s="7" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="46" spans="1:16" ht="51">
@@ -3973,13 +3973,13 @@
         <v>4500</v>
       </c>
       <c r="E46" s="14" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="F46" s="15" t="s">
         <v>127</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="H46" s="15" t="s">
         <v>129</v>
@@ -4009,11 +4009,11 @@
         <v>4600</v>
       </c>
       <c r="E47" s="10" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="F47" s="4"/>
       <c r="G47" s="11" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="H47" s="4" t="s">
         <v>130</v>
@@ -4026,7 +4026,7 @@
         <v>5</v>
       </c>
       <c r="N47" s="7" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="48" spans="1:16" ht="63.75">
@@ -4041,13 +4041,13 @@
         <v>4700</v>
       </c>
       <c r="E48" s="18" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="F48" s="19" t="s">
         <v>132</v>
       </c>
       <c r="G48" s="20" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="H48" s="19" t="s">
         <v>134</v>
@@ -4079,13 +4079,13 @@
         <v>4800</v>
       </c>
       <c r="E49" s="10" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="F49" s="4" t="s">
         <v>112</v>
       </c>
       <c r="G49" s="11" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="H49" s="4" t="s">
         <v>113</v>
@@ -4116,13 +4116,13 @@
         <v>4900</v>
       </c>
       <c r="E50" s="10" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="F50" s="4" t="s">
         <v>87</v>
       </c>
       <c r="G50" s="11" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="H50" s="4" t="s">
         <v>88</v>
@@ -4153,13 +4153,13 @@
         <v>5000</v>
       </c>
       <c r="E51" s="14" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="F51" s="15" t="s">
         <v>137</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="H51" s="15" t="s">
         <v>139</v>
@@ -4189,11 +4189,11 @@
         <v>5100</v>
       </c>
       <c r="E52" s="10" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="F52" s="4"/>
       <c r="G52" s="11" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="H52" s="4" t="s">
         <v>141</v>
@@ -4208,7 +4208,7 @@
         <v>5</v>
       </c>
       <c r="N52" s="7" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="O52" s="7"/>
       <c r="P52" s="6"/>
@@ -4225,13 +4225,13 @@
         <v>5200</v>
       </c>
       <c r="E53" s="10" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="F53" s="4" t="s">
         <v>142</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="H53" s="4" t="s">
         <v>143</v>
@@ -4262,13 +4262,13 @@
         <v>5300</v>
       </c>
       <c r="E54" s="10" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="F54" s="4" t="s">
         <v>142</v>
       </c>
       <c r="G54" s="11" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="H54" s="4" t="s">
         <v>145</v>
@@ -4299,13 +4299,13 @@
         <v>5400</v>
       </c>
       <c r="E55" s="10" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="F55" s="4" t="s">
         <v>142</v>
       </c>
       <c r="G55" s="11" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="H55" s="4" t="s">
         <v>147</v>
@@ -4336,13 +4336,13 @@
         <v>5500</v>
       </c>
       <c r="E56" s="10" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="F56" s="4" t="s">
         <v>142</v>
       </c>
       <c r="G56" s="11" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="H56" s="4" t="s">
         <v>149</v>
@@ -4373,13 +4373,13 @@
         <v>5600</v>
       </c>
       <c r="E57" s="10" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="F57" s="4" t="s">
         <v>142</v>
       </c>
       <c r="G57" s="11" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="H57" s="4" t="s">
         <v>151</v>
@@ -4413,13 +4413,13 @@
         <v>5700</v>
       </c>
       <c r="E58" s="10" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="F58" s="4" t="s">
         <v>153</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="H58" s="4" t="s">
         <v>154</v>
@@ -4452,13 +4452,13 @@
         <v>5800</v>
       </c>
       <c r="E59" s="10" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="F59" s="4" t="s">
         <v>153</v>
       </c>
       <c r="G59" s="11" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="H59" s="4" t="s">
         <v>158</v>
@@ -4486,13 +4486,13 @@
         <v>5900</v>
       </c>
       <c r="E60" s="10" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="F60" s="4" t="s">
         <v>159</v>
       </c>
       <c r="G60" s="11" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="H60" s="4" t="s">
         <v>160</v>
@@ -4522,13 +4522,13 @@
         <v>6000</v>
       </c>
       <c r="E61" s="10" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="F61" s="4" t="s">
         <v>162</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="H61" s="4" t="s">
         <v>163</v>
@@ -4558,13 +4558,13 @@
         <v>6100</v>
       </c>
       <c r="E62" s="10" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="F62" s="4" t="s">
         <v>165</v>
       </c>
       <c r="G62" s="11" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="H62" s="4" t="s">
         <v>166</v>
@@ -4595,13 +4595,13 @@
         <v>6200</v>
       </c>
       <c r="E63" s="10" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="F63" s="4" t="s">
         <v>165</v>
       </c>
       <c r="G63" s="11" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="H63" s="4" t="s">
         <v>167</v>
@@ -4629,13 +4629,13 @@
         <v>6300</v>
       </c>
       <c r="E64" s="10" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="F64" s="4" t="s">
         <v>168</v>
       </c>
       <c r="G64" s="11" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="H64" s="4" t="s">
         <v>169</v>
@@ -4668,13 +4668,13 @@
         <v>6400</v>
       </c>
       <c r="E65" s="10" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="F65" s="4" t="s">
         <v>171</v>
       </c>
       <c r="G65" s="11" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="H65" s="4" t="s">
         <v>172</v>
@@ -4706,13 +4706,13 @@
         <v>6500</v>
       </c>
       <c r="E66" s="10" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="F66" s="4" t="s">
         <v>174</v>
       </c>
       <c r="G66" s="11" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="H66" s="4" t="s">
         <v>175</v>
@@ -4740,13 +4740,13 @@
         <v>6600</v>
       </c>
       <c r="E67" s="10" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="F67" s="4" t="s">
         <v>176</v>
       </c>
       <c r="G67" s="11" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="H67" s="4" t="s">
         <v>177</v>
@@ -4779,13 +4779,13 @@
         <v>6700</v>
       </c>
       <c r="E68" s="10" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="F68" s="4" t="s">
         <v>179</v>
       </c>
       <c r="G68" s="11" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="H68" s="4" t="s">
         <v>180</v>
@@ -4816,13 +4816,13 @@
         <v>6800</v>
       </c>
       <c r="E69" s="10" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="F69" s="4" t="s">
         <v>181</v>
       </c>
       <c r="G69" s="11" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="H69" s="4" t="s">
         <v>182</v>
@@ -4853,13 +4853,13 @@
         <v>6900</v>
       </c>
       <c r="E70" s="10" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="F70" s="4" t="s">
         <v>184</v>
       </c>
       <c r="G70" s="11" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="H70" s="4" t="s">
         <v>185</v>
@@ -4892,13 +4892,13 @@
         <v>7000</v>
       </c>
       <c r="E71" s="10" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="F71" s="4" t="s">
         <v>187</v>
       </c>
       <c r="G71" s="11" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="H71" s="4" t="s">
         <v>188</v>
@@ -4932,13 +4932,13 @@
         <v>7100</v>
       </c>
       <c r="E72" s="10" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="F72" s="4" t="s">
         <v>191</v>
       </c>
       <c r="G72" s="11" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="H72" s="4" t="s">
         <v>192</v>
@@ -4971,13 +4971,13 @@
         <v>7200</v>
       </c>
       <c r="E73" s="10" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="F73" s="4" t="s">
         <v>191</v>
       </c>
       <c r="G73" s="11" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="H73" s="4" t="s">
         <v>195</v>
@@ -5010,13 +5010,13 @@
         <v>7300</v>
       </c>
       <c r="E74" s="10" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="F74" s="4" t="s">
         <v>197</v>
       </c>
       <c r="G74" s="11" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="H74" s="4" t="s">
         <v>198</v>
@@ -5052,13 +5052,13 @@
         <v>7400</v>
       </c>
       <c r="E75" s="10" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="F75" s="4" t="s">
         <v>197</v>
       </c>
       <c r="G75" s="11" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="H75" s="4" t="s">
         <v>202</v>
@@ -5091,13 +5091,13 @@
         <v>7500</v>
       </c>
       <c r="E76" s="10" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="F76" s="4" t="s">
         <v>204</v>
       </c>
       <c r="G76" s="11" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="H76" s="4" t="s">
         <v>205</v>
@@ -5128,13 +5128,13 @@
         <v>7600</v>
       </c>
       <c r="E77" s="10" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="F77" s="4" t="s">
         <v>207</v>
       </c>
       <c r="G77" s="11" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="H77" s="4" t="s">
         <v>208</v>
@@ -5161,13 +5161,13 @@
         <v>7700</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="F78" s="1" t="s">
         <v>211</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="H78" s="15" t="s">
         <v>213</v>
@@ -5191,28 +5191,28 @@
         <v>210</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>215</v>
+        <v>504</v>
       </c>
       <c r="D79" s="13">
         <v>7800</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="F79" s="1" t="s">
         <v>211</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>381</v>
+        <v>505</v>
       </c>
       <c r="H79" s="15" t="s">
+        <v>215</v>
+      </c>
+      <c r="I79" s="15">
+        <v>0</v>
+      </c>
+      <c r="J79" s="16" t="s">
         <v>216</v>
-      </c>
-      <c r="I79" s="15">
-        <v>0</v>
-      </c>
-      <c r="J79" s="16" t="s">
-        <v>217</v>
       </c>
       <c r="M79" s="1">
         <v>3</v>
@@ -5227,28 +5227,28 @@
         <v>210</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D80" s="13">
         <v>7900</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="F80" s="1" t="s">
         <v>211</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="H80" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="I80" s="15">
+        <v>0</v>
+      </c>
+      <c r="J80" s="16" t="s">
         <v>219</v>
-      </c>
-      <c r="I80" s="15">
-        <v>0</v>
-      </c>
-      <c r="J80" s="16" t="s">
-        <v>220</v>
       </c>
       <c r="M80" s="1">
         <v>3</v>
@@ -5265,28 +5265,28 @@
         <v>210</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>221</v>
+        <v>507</v>
       </c>
       <c r="D81" s="13">
         <v>8000</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="F81" s="1" t="s">
         <v>211</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>383</v>
+        <v>506</v>
       </c>
       <c r="H81" s="15" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="I81" s="15">
         <v>0</v>
       </c>
       <c r="J81" s="16" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="M81" s="1">
         <v>3</v>
@@ -5310,22 +5310,22 @@
         <v>8100</v>
       </c>
       <c r="E82" s="10" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="G82" s="11" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="H82" s="4" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="I82" s="4">
         <v>0</v>
       </c>
       <c r="J82" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="M82" s="6">
         <v>3</v>
@@ -5349,16 +5349,16 @@
         <v>8200</v>
       </c>
       <c r="E83" s="10" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="F83" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G83" s="11" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="H83" s="4" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="I83" s="4">
         <v>0</v>
@@ -5379,22 +5379,22 @@
         <v>49</v>
       </c>
       <c r="C84" s="20" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="D84" s="13">
         <v>8300</v>
       </c>
       <c r="E84" s="18" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="F84" s="19" t="s">
+        <v>225</v>
+      </c>
+      <c r="G84" s="20" t="s">
+        <v>382</v>
+      </c>
+      <c r="H84" s="19" t="s">
         <v>227</v>
-      </c>
-      <c r="G84" s="20" t="s">
-        <v>386</v>
-      </c>
-      <c r="H84" s="19" t="s">
-        <v>229</v>
       </c>
       <c r="I84" s="19">
         <v>0</v>
@@ -5422,22 +5422,22 @@
         <v>8400</v>
       </c>
       <c r="E85" s="10" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="F85" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="G85" s="11" t="s">
+        <v>383</v>
+      </c>
+      <c r="H85" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="I85" s="4">
+        <v>0</v>
+      </c>
+      <c r="J85" s="5" t="s">
         <v>230</v>
-      </c>
-      <c r="G85" s="11" t="s">
-        <v>387</v>
-      </c>
-      <c r="H85" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="I85" s="4">
-        <v>0</v>
-      </c>
-      <c r="J85" s="5" t="s">
-        <v>232</v>
       </c>
       <c r="M85" s="6">
         <v>3</v>
@@ -5461,22 +5461,22 @@
         <v>8500</v>
       </c>
       <c r="E86" s="10" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="F86" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="G86" s="11" t="s">
+        <v>384</v>
+      </c>
+      <c r="H86" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="I86" s="4">
+        <v>0</v>
+      </c>
+      <c r="J86" s="5" t="s">
         <v>233</v>
-      </c>
-      <c r="G86" s="11" t="s">
-        <v>388</v>
-      </c>
-      <c r="H86" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="I86" s="4">
-        <v>0</v>
-      </c>
-      <c r="J86" s="5" t="s">
-        <v>235</v>
       </c>
       <c r="M86" s="6">
         <v>4</v>
@@ -5500,22 +5500,22 @@
         <v>8600</v>
       </c>
       <c r="E87" s="10" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="F87" s="4" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="G87" s="11" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="H87" s="4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="I87" s="4">
         <v>0</v>
       </c>
       <c r="J87" s="5" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="M87" s="6">
         <v>4</v>
@@ -5539,22 +5539,22 @@
         <v>8700</v>
       </c>
       <c r="E88" s="10" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="F88" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="G88" s="11" t="s">
+        <v>386</v>
+      </c>
+      <c r="H88" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="I88" s="4">
+        <v>0</v>
+      </c>
+      <c r="J88" s="5" t="s">
         <v>239</v>
-      </c>
-      <c r="G88" s="11" t="s">
-        <v>390</v>
-      </c>
-      <c r="H88" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="I88" s="4">
-        <v>0</v>
-      </c>
-      <c r="J88" s="5" t="s">
-        <v>241</v>
       </c>
       <c r="M88" s="6">
         <v>4</v>
@@ -5578,16 +5578,16 @@
         <v>8800</v>
       </c>
       <c r="E89" s="10" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="F89" s="4" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G89" s="11" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="H89" s="4" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="I89" s="4">
         <v>0</v>
@@ -5615,16 +5615,16 @@
         <v>8900</v>
       </c>
       <c r="E90" s="10" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="F90" s="4" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G90" s="11" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="H90" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="I90" s="4">
         <v>0</v>
@@ -5652,16 +5652,16 @@
         <v>9000</v>
       </c>
       <c r="E91" s="10" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="F91" s="4" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G91" s="11" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="H91" s="4" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="I91" s="4">
         <v>0</v>
@@ -5689,16 +5689,16 @@
         <v>9100</v>
       </c>
       <c r="E92" s="10" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="F92" s="4" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G92" s="11" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="H92" s="4" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="I92" s="4">
         <v>0</v>
@@ -5726,16 +5726,16 @@
         <v>9200</v>
       </c>
       <c r="E93" s="10" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="F93" s="4" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G93" s="11" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H93" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="I93" s="4">
         <v>0</v>
@@ -5760,16 +5760,16 @@
         <v>9300</v>
       </c>
       <c r="E94" s="10" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="F94" s="4" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G94" s="11" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="H94" s="4" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="I94" s="4">
         <v>0</v>
@@ -5794,16 +5794,16 @@
         <v>9400</v>
       </c>
       <c r="E95" s="10" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="F95" s="4" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="G95" s="5" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="H95" s="4" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="I95" s="4">
         <v>0</v>
@@ -5828,16 +5828,16 @@
         <v>9500</v>
       </c>
       <c r="E96" s="10" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="F96" s="4" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="G96" s="11" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="H96" s="4" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="I96" s="4">
         <v>0</v>
@@ -5862,16 +5862,16 @@
         <v>9600</v>
       </c>
       <c r="E97" s="10" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="F97" s="4" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="G97" s="11" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="H97" s="4" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="I97" s="4">
         <v>0</v>
@@ -5881,7 +5881,7 @@
         <v>5</v>
       </c>
       <c r="N97" s="7" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="O97" s="7" t="s">
         <v>209</v>
@@ -5899,16 +5899,16 @@
         <v>9700</v>
       </c>
       <c r="E98" s="10" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="F98" s="4" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="G98" s="11" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="H98" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="I98" s="4">
         <v>0</v>
@@ -5918,7 +5918,7 @@
         <v>5</v>
       </c>
       <c r="N98" s="7" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="O98" s="7" t="s">
         <v>209</v>
@@ -5936,16 +5936,16 @@
         <v>9800</v>
       </c>
       <c r="E99" s="10" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="F99" s="4" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G99" s="11" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="H99" s="4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="I99" s="4">
         <v>0</v>
@@ -5955,7 +5955,7 @@
         <v>5</v>
       </c>
       <c r="N99" s="7" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="O99" s="7" t="s">
         <v>209</v>
@@ -5973,14 +5973,14 @@
         <v>9900</v>
       </c>
       <c r="E100" s="10" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="F100" s="4"/>
       <c r="G100" s="11" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="H100" s="11" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="I100" s="11">
         <v>1</v>
@@ -5992,7 +5992,7 @@
         <v>5</v>
       </c>
       <c r="N100" s="7" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="101" spans="1:16" ht="25.5">
@@ -6007,14 +6007,14 @@
         <v>10000</v>
       </c>
       <c r="E101" s="10" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="F101" s="4"/>
       <c r="G101" s="5" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="H101" s="4" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="I101" s="11">
         <v>1</v>
@@ -6024,7 +6024,7 @@
         <v>5</v>
       </c>
       <c r="N101" s="7" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="102" spans="1:16" s="23" customFormat="1" ht="25.5">
@@ -6039,14 +6039,14 @@
         <v>10100</v>
       </c>
       <c r="E102" s="10" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="F102" s="4"/>
       <c r="G102" s="11" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="H102" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="I102" s="11">
         <v>1</v>
@@ -6058,7 +6058,7 @@
         <v>5</v>
       </c>
       <c r="N102" s="7" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="O102" s="7"/>
       <c r="P102" s="6"/>
@@ -6075,14 +6075,14 @@
         <v>10200</v>
       </c>
       <c r="E103" s="10" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="F103" s="4"/>
       <c r="G103" s="11" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="H103" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="I103" s="11">
         <v>1</v>
@@ -6092,11 +6092,11 @@
         <v>5</v>
       </c>
       <c r="N103" s="7" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="O103" s="22"/>
       <c r="P103" s="6" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="104" spans="1:16" ht="38.25">
@@ -6111,14 +6111,14 @@
         <v>10300</v>
       </c>
       <c r="E104" s="10" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="F104" s="4"/>
       <c r="G104" s="5" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="H104" s="4" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="I104" s="11">
         <v>1</v>
@@ -6128,7 +6128,7 @@
         <v>5</v>
       </c>
       <c r="N104" s="7" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="105" spans="1:16" ht="38.25">
@@ -6143,14 +6143,14 @@
         <v>10400</v>
       </c>
       <c r="E105" s="10" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="F105" s="4"/>
       <c r="G105" s="11" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="H105" s="4" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="I105" s="11">
         <v>1</v>
@@ -6160,7 +6160,7 @@
         <v>5</v>
       </c>
       <c r="N105" s="7" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="106" spans="1:16" ht="38.25">
@@ -6175,14 +6175,14 @@
         <v>10500</v>
       </c>
       <c r="E106" s="10" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="F106" s="4"/>
       <c r="G106" s="11" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="H106" s="4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I106" s="11">
         <v>1</v>
@@ -6192,7 +6192,7 @@
         <v>5</v>
       </c>
       <c r="N106" s="7" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="107" spans="1:16" ht="51">
@@ -6207,14 +6207,14 @@
         <v>10600</v>
       </c>
       <c r="E107" s="10" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="F107" s="4"/>
       <c r="G107" s="11" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="H107" s="4" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="I107" s="11">
         <v>1</v>
@@ -6224,13 +6224,13 @@
         <v>5</v>
       </c>
       <c r="N107" s="7" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="O107" s="7" t="s">
         <v>57</v>
       </c>
       <c r="P107" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="108" spans="1:16" ht="51">
@@ -6245,14 +6245,14 @@
         <v>10700</v>
       </c>
       <c r="E108" s="10" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="F108" s="4"/>
       <c r="G108" s="11" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="H108" s="4" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="I108" s="11">
         <v>1</v>
@@ -6262,7 +6262,7 @@
         <v>5</v>
       </c>
       <c r="N108" s="7" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="O108" s="7" t="s">
         <v>57</v>
@@ -6280,14 +6280,14 @@
         <v>10800</v>
       </c>
       <c r="E109" s="10" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="F109" s="4"/>
       <c r="G109" s="11" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="H109" s="4" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="I109" s="11">
         <v>1</v>
@@ -6297,7 +6297,7 @@
         <v>5</v>
       </c>
       <c r="N109" s="7" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="O109" s="7" t="s">
         <v>57</v>
@@ -6305,37 +6305,37 @@
     </row>
     <row r="110" spans="1:16" s="1" customFormat="1" ht="102">
       <c r="A110" s="14" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D110" s="13">
         <v>10900</v>
       </c>
       <c r="E110" s="14" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="F110" s="15" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="G110" s="1" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="H110" s="15" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="I110" s="15">
         <v>0</v>
       </c>
       <c r="J110" s="16" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="M110" s="1">
         <v>5</v>
       </c>
       <c r="N110" s="15" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="O110" s="15" t="s">
         <v>209</v>
@@ -6343,116 +6343,116 @@
     </row>
     <row r="111" spans="1:16" s="1" customFormat="1" ht="89.25">
       <c r="A111" s="14" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D111" s="13">
         <v>11000</v>
       </c>
       <c r="E111" s="14" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="F111" s="15" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="G111" s="1" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="H111" s="15" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="I111" s="15">
         <v>0</v>
       </c>
       <c r="J111" s="16" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="M111" s="1">
         <v>5</v>
       </c>
       <c r="N111" s="15" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="O111" s="15" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="112" spans="1:16" s="1" customFormat="1" ht="89.25">
       <c r="A112" s="14" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D112" s="13">
         <v>11100</v>
       </c>
       <c r="E112" s="14" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="F112" s="15" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="G112" s="1" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="H112" s="15" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="I112" s="15">
         <v>0</v>
       </c>
       <c r="J112" s="16" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="M112" s="1">
         <v>5</v>
       </c>
       <c r="N112" s="15" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="O112" s="15" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="113" spans="1:16" s="1" customFormat="1" ht="89.25">
       <c r="A113" s="14" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D113" s="13">
         <v>11200</v>
       </c>
       <c r="E113" s="14" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="F113" s="15" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="G113" s="1" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="H113" s="15" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="I113" s="15">
         <v>0</v>
       </c>
       <c r="J113" s="16" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="M113" s="1">
         <v>5</v>
       </c>
       <c r="N113" s="15" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="O113" s="15" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="114" spans="1:16" ht="25.5">
@@ -6467,14 +6467,14 @@
         <v>11300</v>
       </c>
       <c r="E114" s="10" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="F114" s="4"/>
       <c r="G114" s="11" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="H114" s="11" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="I114" s="11">
         <v>1</v>
@@ -6486,11 +6486,11 @@
         <v>5</v>
       </c>
       <c r="N114" s="7" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="O114" s="22"/>
       <c r="P114" s="6" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="115" spans="1:16" ht="51">
@@ -6505,16 +6505,16 @@
         <v>11400</v>
       </c>
       <c r="E115" s="10" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="F115" s="4" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="G115" s="11" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="H115" s="4" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="I115" s="4">
         <v>0</v>
@@ -6542,16 +6542,16 @@
         <v>11500</v>
       </c>
       <c r="E116" s="10" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="F116" s="4" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="G116" s="11" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="H116" s="4" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="I116" s="4">
         <v>0</v>
@@ -6582,16 +6582,16 @@
         <v>11600</v>
       </c>
       <c r="E117" s="10" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="F117" s="4" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="G117" s="11" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="H117" s="4" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="I117" s="4">
         <v>0</v>
@@ -6619,14 +6619,14 @@
         <v>11700</v>
       </c>
       <c r="E118" s="10" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="F118" s="4"/>
       <c r="G118" s="11" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="H118" s="4" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="I118" s="11">
         <v>1</v>
@@ -6638,7 +6638,7 @@
         <v>5</v>
       </c>
       <c r="N118" s="7" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="119" spans="1:16" ht="51">
@@ -6653,16 +6653,16 @@
         <v>11800</v>
       </c>
       <c r="E119" s="10" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="F119" s="4" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="G119" s="11" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="H119" s="4" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="I119" s="4">
         <v>0</v>
@@ -6690,16 +6690,16 @@
         <v>11900</v>
       </c>
       <c r="E120" s="10" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="F120" s="4" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="G120" s="11" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="H120" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="I120" s="4">
         <v>0</v>
@@ -6730,14 +6730,14 @@
         <v>12000</v>
       </c>
       <c r="E121" s="10" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="F121" s="4"/>
       <c r="G121" s="11" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="H121" s="11" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="I121" s="11">
         <v>1</v>
@@ -6749,7 +6749,7 @@
         <v>5</v>
       </c>
       <c r="N121" s="7" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="122" spans="1:16" ht="51">
@@ -6764,16 +6764,16 @@
         <v>12100</v>
       </c>
       <c r="E122" s="10" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="F122" s="4" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="G122" s="11" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="H122" s="4" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="I122" s="4">
         <v>0</v>
@@ -6801,16 +6801,16 @@
         <v>12200</v>
       </c>
       <c r="E123" s="10" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="F123" s="4" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="G123" s="11" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="H123" s="4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="I123" s="4">
         <v>0</v>

</xml_diff>